<commit_message>
update pipline and add plot process
</commit_message>
<xml_diff>
--- a/src/out/all-preprocessed.xlsx
+++ b/src/out/all-preprocessed.xlsx
@@ -497,7 +497,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,online bank,distribute database,database system,cryptography,tutorial</t>
+          <t>peer-to-peer,online bank,distribute database,database system,cryptography,tutorial</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>data mine,peer-to-peer compute,cryptography,internet,online bank,contract,bibliography</t>
+          <t>data mine,peer-to-peer,cryptography,internet,online bank,contract,bibliography</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>bitcoin,ethereum,smart contract,cryptography,distribute database,advance configuration,power interface,authentication,parity bite</t>
+          <t>bitcoin,ethereum,contract,cryptography,distribute database,advance configuration,power interface,authentication,parity bite</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>microgrids,bitcoin,contract,process control,renewable energy source,peer-to-peer compute</t>
+          <t>microgrids,bitcoin,contract,process control,renewable energy source,peer-to-peer</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>bitcoin,peer-to-peer compute,organization,contract</t>
+          <t>bitcoin,peer-to-peer,organization,contract</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>protocol,peer-to-peer compute,contract,bitcoin,fault tolerance,fault tolerant system,law</t>
+          <t>protocol,peer-to-peer,contract,bitcoin,fault tolerance,fault tolerant system,law</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>algorithm design,analysis,bitcoin,peer-to-peer compute,server,safety,fault tolerance</t>
+          <t>algorithm design,analysis,bitcoin,peer-to-peer,server,safety,fault tolerance</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,medical service,bitcoin,industry,electrical engineer</t>
+          <t>peer-to-peer,medical service,bitcoin,industry,electrical engineer</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>contract,peer-to-peer compute,security,monitor,smart home,intelligent sensor</t>
+          <t>contract,peer-to-peer,security,monitor,smart home,intelligent sensor</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>bitcoin,peer-to-peer compute,bank,elliptic curve cryptography</t>
+          <t>bitcoin,peer-to-peer,bank,elliptic curve cryptography</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>blockchain,research framework,review,distributed ledger technology,digitalization</t>
+          <t>blockchain,research framework,review,distribute ledger,digitalization</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>bitcoin,smart contract,data integrity,open research,spectral leakage,extravasation,information privacy</t>
+          <t>bitcoin,contract,data integrity,open research,spectral leakage,extravasation,information privacy</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>bitcoin,software developer,open-source software,internet of things,software engineer,debugger,identity management,software development,smart contract,integrate development environment,primary source,program tool,simulation,ecosystem</t>
+          <t>bitcoin,software developer,open-source software,internet of things,software engineer,debugger,identity management,software development,contract,integrate development environment,primary source,program tool,simulation,ecosystem</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,smart contract,privacy</t>
+          <t>bitcoin,cryptocurrency,contract,privacy</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,ride-hailing service,secure bill</t>
+          <t>contract,blockchain,ride-hailing service,secure bill</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>blockchain,bank,peer-to-peer compute,contract,finance,distribute database</t>
+          <t>blockchain,bank,peer-to-peer,contract,finance,distribute database</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>intrusion detection,peer-to-peer compute,bitcoin</t>
+          <t>intrusion detection,peer-to-peer,bitcoin</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,blockchain,biological system model,computational model,server,bay method,bitcoin</t>
+          <t>peer-to-peer,blockchain,biological system model,computational model,server,bay method,bitcoin</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>blockchain,internet of things,bitcoin,government,distribute ledger,peer-to-peer compute</t>
+          <t>blockchain,internet of things,bitcoin,government,distribute ledger,peer-to-peer</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>bitcoin,blockchain,peer-to-peer compute,receiver,server,public key</t>
+          <t>bitcoin,blockchain,peer-to-peer,receiver,server,public key</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3406,7 +3406,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>blockchain,peer-to-peer compute,computer security,bitcoin,authorization,smart contract</t>
+          <t>blockchain,peer-to-peer,computer security,bitcoin,authorization,contract</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3449,7 +3449,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>blockchain,bitcoin,internet of things,systematics,smart contract,distribute ledger,library</t>
+          <t>blockchain,bitcoin,internet of things,systematics,contract,distribute ledger,library</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,peer-to-peer compute,cryptography,distribute database,digital forensics</t>
+          <t>blockchain,contract,peer-to-peer,cryptography,distribute database,digital forensics</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>blockchain,security,technology,smart contract,consensus</t>
+          <t>blockchain,security,technology,contract,consensus</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,urban area,bitcoin,bibliography,sustainable development</t>
+          <t>peer-to-peer,urban area,bitcoin,bibliography,sustainable development</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3707,7 +3707,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>cryptography,digital signature,internet of things,peer-to-peer compute,big data</t>
+          <t>cryptography,digital signature,internet of things,peer-to-peer,big data</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,bitcoin,internet of things,cloud compute,computer architecture</t>
+          <t>peer-to-peer,bitcoin,internet of things,cloud compute,computer architecture</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>bitcoin,peer-to-peer compute,software,server</t>
+          <t>bitcoin,peer-to-peer,software,server</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>intrusion detection,collaboration,peer-to-peer compute,monitor,resistance</t>
+          <t>intrusion detection,collaboration,peer-to-peer,monitor,resistance</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>bitcoin,privacy,peer-to-peer compute,proposal,history</t>
+          <t>bitcoin,privacy,peer-to-peer,proposal,history</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -4267,7 +4267,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>legal contract,smart contract,blockchain</t>
+          <t>legal contract,contract,blockchain</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -4716,7 +4716,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>blockchain,smart grid,smart contract,energy sector,electric utility,business process innovation,energy transformation</t>
+          <t>blockchain,smart grid,contract,energy sector,electric utility,business process innovation,energy transformation</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -4805,7 +4805,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,dapp,architecture style,software architecture,internet of things</t>
+          <t>blockchain,contract,dapp,architecture style,software architecture,internet of things</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -5064,7 +5064,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>smart place,blockchain,review,internet of things,smart contract,e-governance</t>
+          <t>smart place,blockchain,review,internet of things,contract,e-governance</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>blockchain,cyber attack,cryptocurrency exchange,ico,smart contract</t>
+          <t>blockchain,cyber attack,cryptocurrency exchange,ico,contract</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -5455,7 +5455,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>blockchain,blockchain,crypto-spatial coordinate system,cryptography,distributed ledger technology,smart contract,internet of things,smart city,clinical trial,supply chain,pharmaceutical,healthcare</t>
+          <t>blockchain,blockchain,crypto-spatial coordinate system,cryptography,distribute ledger,contract,internet of things,smart city,clinical trial,supply chain,pharmaceutical,healthcare</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>blockchain,distribute ledger,smart contract,healthcare,patient,security</t>
+          <t>blockchain,distribute ledger,contract,healthcare,patient,security</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -5805,7 +5805,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t xml:space="preserve">bitcoin ,technology,smart contract,consensus,elliptic curve digital signature algorithm </t>
+          <t xml:space="preserve">bitcoin ,technology,contract,consensus,elliptic curve digital signature algorithm </t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -5891,7 +5891,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,construction industry,build environment,socio-technical system</t>
+          <t>blockchain,distribute ledger,construction industry,build environment,socio-technical system</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology</t>
+          <t>blockchain,distribute ledger</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -6236,7 +6236,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>smart contract,business process,trust third party,categorization,embed system</t>
+          <t>contract,business process,trust third party,categorization,embed system</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -6409,7 +6409,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t xml:space="preserve">bitcoin,cloud compute,next-generation network,internet of things,program paradigm,information privacy,cyber security,scalability,smart city,elasticity </t>
+          <t xml:space="preserve">bitcoin,cloud compute,next-generation network,internet of things,program paradigm,information privacy,security,scalability,smart city,elasticity </t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6495,7 +6495,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>smart contract,ethereum,best practice,business logic,encode,bitcoin</t>
+          <t>contract,ethereum,best practice,business logic,encode,bitcoin</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -6538,7 +6538,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>ethereum,smart contract,formal verification,vulnerability ,cryptocurrency,application security,solidity,arithmetic underflow,correctness ,distribute compute,computer data storage,categorization,autonomous robot,malware,code,signature block,h,y board,data access object</t>
+          <t>ethereum,contract,formal verification,vulnerability ,cryptocurrency,application security,solidity,arithmetic underflow,correctness ,distribute compute,computer data storage,categorization,autonomous robot,malware,code,signature block,h,y board,data access object</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -6581,7 +6581,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>zero-knowledge proof,cryptography,distributed ledger technology</t>
+          <t>zero-knowledge proof,cryptography,distribute ledger</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -6710,7 +6710,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,business process,behavior,apathy,gene regulatory network,genie,cryptosporidiosis,distributed ledger technology,capacity build</t>
+          <t>bitcoin,cryptocurrency,business process,behavior,apathy,gene regulatory network,genie,cryptosporidiosis,distribute ledger,capacity build</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -6753,7 +6753,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>smart contract,ethereum,software bug,design by contract,immutable object,bitcoin,patch ,computer performance,stack exchange,categorization,flaw hypothesis methodology,software deployment</t>
+          <t>contract,ethereum,software bug,design by contract,immutable object,bitcoin,patch ,computer performance,stack exchange,categorization,flaw hypothesis methodology,software deployment</t>
         </is>
       </c>
       <c r="E146" t="inlineStr"/>
@@ -7050,7 +7050,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,privacy,cryptography,internet of things,smart contract,non-interactive zero-knowledge proof,computer security,e-commerce,interactivity,requirement,antivirus software,algorithm</t>
+          <t>bitcoin,cryptocurrency,privacy,cryptography,internet of things,contract,non-interactive zero-knowledge proof,computer security,e-commerce,interactivity,requirement,antivirus software,algorithm</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -7136,7 +7136,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t xml:space="preserve">smart contract,ethereum,datalog,bitcoin,vulnerability ,trace </t>
+          <t xml:space="preserve">contract,ethereum,datalog,bitcoin,vulnerability ,trace </t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -7265,7 +7265,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>ethereum,smart contract,solidity,vulnerability ,debug,run time ,extensibility</t>
+          <t>ethereum,contract,solidity,vulnerability ,debug,run time ,extensibility</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -7351,7 +7351,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>machine learn,bitcoin,reinforcement learn,artificial intelligence,big data</t>
+          <t>machine learning,bitcoin,reinforcement learn,artificial intelligence,big data</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -7394,7 +7394,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>bitcoin,immutable object,right to be forget,requirement,smart contract,cryptography,general data protection regulation</t>
+          <t>bitcoin,immutable object,right to be forget,requirement,contract,cryptography,general data protection regulation</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>internet of things,bitcoin,information privacy,requirement,interoperability,encryption,scalability,information silo,centralize compute,smart contract,mechatronics,st,ards characteristic,cryptography,distribute database,computer security,floor,ceiling function,high- and low-level,protocol documentation,embed system,overhead ,server ,solution,contract agreement,node - plant part,physical object,convergence ,embed,genetic heterogeneity</t>
+          <t>internet of things,bitcoin,information privacy,requirement,interoperability,encryption,scalability,information silo,centralize compute,contract,mechatronics,st,ards characteristic,cryptography,distribute database,computer security,floor,ceiling function,high- and low-level,protocol documentation,embed system,overhead ,server ,solution,contract agreement,node - plant part,physical object,convergence ,embed,genetic heterogeneity</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -7652,7 +7652,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>industry 4.0,bitcoin,robotics,smart contract,big data,internet of things</t>
+          <t>industry,bitcoin,robotics,contract,big data,internet of things</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -7734,7 +7734,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t xml:space="preserve">attack surface,bitcoin,denial-of-service attack,smart contract,distribute compute,causality,context ,cryptography,nervous system disorder,theft,lope gorlin syndrome,cutlery fork,domain name,contribution,denial </t>
+          <t xml:space="preserve">attack surface,bitcoin,denial-of-service attack,contract,distribute compute,causality,context ,cryptography,nervous system disorder,theft,lope gorlin syndrome,cutlery fork,domain name,contribution,denial </t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -7820,7 +7820,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>blockchain,cryptocurrency,mine,smart contract,security,privacy</t>
+          <t>blockchain,cryptocurrency,mine,contract,security,privacy</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -7863,7 +7863,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,cyber security,distributed ledger technology,internet of things,cryptocurrency,bitcoin</t>
+          <t>blockchain,contract,security,distribute ledger,internet of things,cryptocurrency,bitcoin</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -8164,7 +8164,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>ontological completeness,esml,socio-technical,legal relevance,antlr,blockchain,smart contract</t>
+          <t>ontological completeness,esml,socio-technical,legal relevance,antlr,blockchain,contract</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -8294,7 +8294,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>smart contract,digital economy,blockchain</t>
+          <t>contract,digital economy,blockchain</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -8337,7 +8337,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,electronic document,taxation</t>
+          <t>blockchain,contract,electronic document,taxation</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -8423,7 +8423,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>smart contract,technology,islamic trade finance,digital bank,islamic finance</t>
+          <t>contract,technology,islamic trade finance,digital bank,islamic finance</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -8512,7 +8512,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,application,legislation,colombia</t>
+          <t>blockchain,contract,application,legislation,colombia</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -8599,7 +8599,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>bitcoin,blockchain,peer-to-peer compute,ip network</t>
+          <t>bitcoin,blockchain,peer-to-peer,ip network</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -9156,7 +9156,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>blockchain,bitcoin,tutorial,peer-to-peer compute,public key,conference</t>
+          <t>blockchain,bitcoin,tutorial,peer-to-peer,public key,conference</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -9457,7 +9457,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,systematics,cryptography,education,bibliography</t>
+          <t>blockchain,contract,systematics,cryptography,education,bibliography</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -9543,7 +9543,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>blockchain,oil,natural gas industry,peer-to-peer compute,natural gas,security,distribute database</t>
+          <t>blockchain,oil,natural gas industry,peer-to-peer,natural gas,security,distribute database</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -9586,7 +9586,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>blockchain,peer-to-peer compute,computer crime,authentication,bitcoin</t>
+          <t>blockchain,peer-to-peer,computer crime,authentication,bitcoin</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -9672,7 +9672,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>blockchain,protocol,game,game theory,cryptography,peer-to-peer compute</t>
+          <t>blockchain,protocol,game,game theory,cryptography,peer-to-peer</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -9887,7 +9887,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>blockchain,industry,organization,cryptography,smart contract</t>
+          <t>blockchain,industry,organization,cryptography,contract</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>blockchain,peer-to-peer compute,privacy,digital signature,information technology,consensus</t>
+          <t>blockchain,peer-to-peer,privacy,digital signature,information technology,consensus</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
@@ -9973,7 +9973,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>blockchain,peer-to-peer compute,consensus,protocol,bitcoin,fabric</t>
+          <t>blockchain,peer-to-peer,consensus,protocol,bitcoin,fabric</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
@@ -10016,7 +10016,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>blockchain,edge compute,bitcoin,peer-to-peer compute,scalability,cloud compute</t>
+          <t>blockchain,edge compute,bitcoin,peer-to-peer,scalability,cloud compute</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -10059,7 +10059,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,machine learn,decision make,machine learn algorithm,data mine</t>
+          <t>blockchain,contract,machine learning,decision make,machine learn algorithm,data mine</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -10102,7 +10102,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>blockchain,computer architecture,smart contract,government,cloud compute,systematics,bitcoin</t>
+          <t>blockchain,computer architecture,contract,government,cloud compute,systematics,bitcoin</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
@@ -10188,7 +10188,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>government,industry,peer-to-peer compute,contract</t>
+          <t>government,industry,peer-to-peer,contract</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,security,law,reliability,taxonomy</t>
+          <t>contract,blockchain,security,law,reliability,taxonomy</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
@@ -10278,7 +10278,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>blockchain,bitcoin,peer-to-peer compute,digital signature,computer architecture,government</t>
+          <t>blockchain,bitcoin,peer-to-peer,digital signature,computer architecture,government</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
@@ -10321,7 +10321,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>industry,medical service,peer-to-peer compute,internet of things,contract,production</t>
+          <t>industry,medical service,peer-to-peer,internet of things,contract,production</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
@@ -10364,7 +10364,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>blockchain,internet of things,security,peer-to-peer compute,data collection,database,smart contract</t>
+          <t>blockchain,internet of things,security,peer-to-peer,data collection,database,contract</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -10450,7 +10450,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>blockchain,bitcoin,smart contract,peer-to-peer compute,internet of things</t>
+          <t>blockchain,bitcoin,contract,peer-to-peer,internet of things</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
@@ -10493,7 +10493,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>blockchain,peer-to-peer compute,digital signature,bitcoin,public key,task analysis</t>
+          <t>blockchain,peer-to-peer,digital signature,bitcoin,public key,task analysis</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -10622,7 +10622,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>smart city,blockchain,security,sociology,statistic,peer-to-peer compute</t>
+          <t>smart city,blockchain,security,sociology,statistic,peer-to-peer</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
@@ -10665,7 +10665,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>blockchain,bitcoin,consensus,peer-to-peer compute,scalability,market research</t>
+          <t>blockchain,bitcoin,consensus,peer-to-peer,scalability,market research</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -10794,7 +10794,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>blockchain,bitcoin,peer-to-peer compute,proof-of-work,smart contract</t>
+          <t>blockchain,bitcoin,peer-to-peer,proof-of-work,contract</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
@@ -10966,7 +10966,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>blockchain,consensus,peer-to-peer compute,classification algorithm,bitcoin,database</t>
+          <t>blockchain,consensus,peer-to-peer,classification algorithm,bitcoin,database</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
@@ -11009,7 +11009,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,internet of things,cloud compute,cryptography,medical service</t>
+          <t>peer-to-peer,internet of things,cloud compute,cryptography,medical service</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
@@ -11052,7 +11052,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>blockchain,industry,smart contract,art,technological innovation</t>
+          <t>blockchain,industry,contract,art,technological innovation</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
@@ -11095,7 +11095,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,computational model,model check,syntactics</t>
+          <t>contract,blockchain,computational model,model check,syntactics</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -11138,7 +11138,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>cloud compute,blockchain,edge compute,smart contract,computer architecture,internet of things,control system</t>
+          <t>cloud compute,blockchain,edge compute,contract,computer architecture,internet of things,control system</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -11224,7 +11224,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>blockchain,stakeholder,smart contract,cryptography,peer-to-peer compute</t>
+          <t>blockchain,stakeholder,contract,cryptography,peer-to-peer</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>microgrids,power market,blockchain,power system stability,peer-to-peer compute,distribute power generation</t>
+          <t>microgrids,power market,blockchain,power system stability,peer-to-peer,distribute power generation</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
@@ -11740,7 +11740,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,peer-to-peer compute,systematics,bitcoin</t>
+          <t>contract,blockchain,peer-to-peer,systematics,bitcoin</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
@@ -11783,7 +11783,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,hardware architecture,review,consensus,heterogeneous hardware,fpga,gpu,asic,cpu</t>
+          <t>blockchain,distribute ledger,hardware architecture,review,consensus,heterogeneous hardware,fpga,gpu,asic,cpu</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
@@ -11869,7 +11869,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>blockchain,protocol,peer-to-peer compute,bitcoin,history,privacy</t>
+          <t>blockchain,protocol,peer-to-peer,bitcoin,history,privacy</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
@@ -11912,7 +11912,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,bitcoin,blockchain,explosive,online bank,ip network</t>
+          <t>peer-to-peer,bitcoin,blockchain,explosive,online bank,ip network</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
@@ -11955,7 +11955,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>protocol,blockchain,distribute ledger,peer-to-peer compute,fault tolerance,fault tolerant system,systematics</t>
+          <t>protocol,blockchain,distribute ledger,peer-to-peer,fault tolerance,fault tolerant system,systematics</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
@@ -12041,7 +12041,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>blockchain,radiology,bitcoin,ethereum,machine learn</t>
+          <t>blockchain,radiology,bitcoin,ethereum,machine learning</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
@@ -12084,7 +12084,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>ips2,blockchain,smart contract</t>
+          <t>ips2,blockchain,contract</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -12342,7 +12342,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>blockchain,data management,smart contract,consensus,data share</t>
+          <t>blockchain,data management,contract,consensus,data share</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -12644,7 +12644,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,healthcare technology,health informatics,supply chain,clinical trial,medical licensure,genomics,electronic health record</t>
+          <t>blockchain,distribute ledger,healthcare technology,health informatics,supply chain,clinical trial,medical licensure,genomics,electronic health record</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -12865,7 +12865,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>distribute ledger,blockchain,smart contract,ethereum,access control,xacml</t>
+          <t>distribute ledger,blockchain,contract,ethereum,access control,xacml</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -13037,7 +13037,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>coordination,smart contract,linda on ethereum,linda on fabric,linda on corda</t>
+          <t>coordination,contract,linda on ethereum,linda on fabric,linda on corda</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -13166,7 +13166,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>ethereum,smart contract,sealed-bid auction</t>
+          <t>ethereum,contract,sealed-bid auction</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -13468,7 +13468,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>blockchain,artificial intelligence,deep learning,machine learn,encryption,decentralize consensus,ethereum,hyperledger,electronic medical record,emr,pharma,insurance,health information exchange,internet of things,pharmacogenomics,robotics,precision medicine</t>
+          <t>blockchain,artificial intelligence,deep learning,machine learning,encryption,decentralize consensus,ethereum,hyperledger,electronic medical record,emr,pharma,insurance,health information exchange,internet of things,pharmacogenomics,robotics,precision medicine</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -13730,7 +13730,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>blockchain,cybercrime,cyber security,healthcare,critical national infrastructure ,scada,threat factor,red team,cyberwarfare,data breach,cyber operation</t>
+          <t>blockchain,cybercrime,security,healthcare,critical national infrastructure ,scada,threat factor,red team,cyberwarfare,data breach,cyber operation</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -13816,7 +13816,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>aesthetic,blockchain,smart contract,critical technical practice,interactional aesthetic</t>
+          <t>aesthetic,blockchain,contract,critical technical practice,interactional aesthetic</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -13946,7 +13946,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>blockchain,cryptocurrency,bitcoin,smart contract,microgrid,distribute ledger,distribute mobility service,autonomous vehicle,ridesharing,renewable energy,distribute generation,photovoltaic,electric vehicle,solar energy,electric grid</t>
+          <t>blockchain,cryptocurrency,bitcoin,contract,microgrid,distribute ledger,distribute mobility service,autonomous vehicle,ridesharing,renewable energy,distribute generation,photovoltaic,electric vehicle,solar energy,electric grid</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
@@ -14033,7 +14033,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>industrial iot,industry 4.0,industry 4.0,blockchain,cyber security,supply chain,data privacy,cryptography</t>
+          <t>industrial iot,industry,industry,blockchain,security,supply chain,data privacy,cryptography</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -14817,7 +14817,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>blockchain,decentralize,peer-to-peer,distribute ledger,smart contract,pharmaceutical supply chain</t>
+          <t>blockchain,decentralize,peer-to-peer,distribute ledger,contract,pharmaceutical supply chain</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
@@ -14860,7 +14860,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>blockchain,artificial intelligence,decentralize network,cryptocurrency,machine learn,deep learning</t>
+          <t>blockchain,artificial intelligence,decentralize network,cryptocurrency,machine learning,deep learning</t>
         </is>
       </c>
       <c r="E334" t="inlineStr">
@@ -14947,7 +14947,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>blockchain,anomaly detection,data mine,graph analysis,cyber security</t>
+          <t>blockchain,anomaly detection,data mine,graph analysis,security</t>
         </is>
       </c>
       <c r="E336" t="inlineStr">
@@ -15121,7 +15121,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>technology,healthcare,electronic health record ,distributed ledger technology,security,privacy-preserving,decentralise application</t>
+          <t>technology,healthcare,electronic health record ,distribute ledger,security,privacy-preserving,decentralise application</t>
         </is>
       </c>
       <c r="E340" t="inlineStr">
@@ -15253,7 +15253,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>blockchain,cyber security,cyber attack,network supervision</t>
+          <t>blockchain,security,cyber attack,network supervision</t>
         </is>
       </c>
       <c r="E343" t="inlineStr">
@@ -15867,7 +15867,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,conceptualization,terminology,technology adoption,o39</t>
+          <t>blockchain,distribute ledger,conceptualization,terminology,technology adoption,o39</t>
         </is>
       </c>
       <c r="E357" t="inlineStr">
@@ -16045,7 +16045,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,project ecosystem,technical,legal issue</t>
+          <t>blockchain,contract,project ecosystem,technical,legal issue</t>
         </is>
       </c>
       <c r="E361" t="inlineStr">
@@ -16313,7 +16313,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>blockchain,byzantine fault tolerance,distributed ledger technology,bitcoin,distribute system</t>
+          <t>blockchain,byzantine fault tolerance,distribute ledger,bitcoin,distribute system</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
@@ -16399,7 +16399,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>smart contract,software engineer,blockchain</t>
+          <t>contract,software engineer,blockchain</t>
         </is>
       </c>
       <c r="E369" t="inlineStr">
@@ -16531,7 +16531,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>blockchain,security,internet of things,smart contract,artificial intelligence,cloud compute</t>
+          <t>blockchain,security,internet of things,contract,artificial intelligence,cloud compute</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
@@ -16747,7 +16747,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,distribute system,internet of things,security</t>
+          <t>blockchain,distribute ledger,distribute system,internet of things,security</t>
         </is>
       </c>
       <c r="E377" t="inlineStr">
@@ -17311,7 +17311,7 @@
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>blockchain,cryptocurrency,electronic payment,decentralize payment system,mine,energy efficiency,bitcoin,ethereum,monero,smart contract,ransomware,profitability</t>
+          <t>blockchain,cryptocurrency,electronic payment,decentralize payment system,mine,energy efficiency,bitcoin,ethereum,monero,contract,ransomware,profitability</t>
         </is>
       </c>
       <c r="E390" t="inlineStr">
@@ -17354,7 +17354,7 @@
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,use case</t>
+          <t>blockchain,contract,use case</t>
         </is>
       </c>
       <c r="E391" t="inlineStr">
@@ -17700,7 +17700,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t xml:space="preserve">smart contract,formal specification,formal verification,verification,validation,computer program,bitcoin,correctness </t>
+          <t xml:space="preserve">contract,formal specification,formal verification,verification,validation,computer program,bitcoin,correctness </t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -17786,7 +17786,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>smart contract,ethereum,review,ecosystem</t>
+          <t>contract,ethereum,review,ecosystem</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -17915,7 +17915,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>ethereum,self-destruct,smart contract,vector ,sensor</t>
+          <t>ethereum,self-destruct,contract,vector ,sensor</t>
         </is>
       </c>
       <c r="E404" t="inlineStr">
@@ -18090,7 +18090,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>machine learn,privacy,internet of things,algorithm,bitcoin,categorization,database</t>
+          <t>machine learning,privacy,internet of things,algorithm,bitcoin,categorization,database</t>
         </is>
       </c>
       <c r="E408" t="inlineStr"/>
@@ -18211,7 +18211,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,focus group,smart contract,centralize compute,librarian,money,formal verification,entity</t>
+          <t>bitcoin,cryptocurrency,focus group,contract,centralize compute,librarian,money,formal verification,entity</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -18512,7 +18512,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>bitcoin,concept map,smart contract,review,digital electronics</t>
+          <t>bitcoin,concept map,contract,review,digital electronics</t>
         </is>
       </c>
       <c r="E418" t="inlineStr">
@@ -18766,7 +18766,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>artificial intelligence,technological convergence,scope ,distributed ledger technology,review,lively kernel</t>
+          <t>artificial intelligence,technological convergence,scope ,distribute ledger,review,lively kernel</t>
         </is>
       </c>
       <c r="E424" t="inlineStr">
@@ -18981,7 +18981,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>blockchain,sidechains,smart contract,decentralize application,decentralize ledger,digital asset,cryptocurrency</t>
+          <t>blockchain,sidechains,contract,decentralize application,decentralize ledger,digital asset,cryptocurrency</t>
         </is>
       </c>
       <c r="E429" t="inlineStr">
@@ -19024,7 +19024,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,smart contract,distribute application</t>
+          <t>blockchain,distribute ledger,contract,distribute application</t>
         </is>
       </c>
       <c r="E430" t="inlineStr">
@@ -19110,7 +19110,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,verification,correctness,security assurance</t>
+          <t>contract,blockchain,verification,correctness,security assurance</t>
         </is>
       </c>
       <c r="E432" t="inlineStr">
@@ -19282,7 +19282,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t xml:space="preserve">smart contract,development process model,software engineer,blockchain,distributed ledger technology,survey,design science,trustless append-only decentralize digital ledger </t>
+          <t xml:space="preserve">contract,development process model,software engineer,blockchain,distribute ledger,survey,design science,trustless append-only decentralize digital ledger </t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
@@ -19457,7 +19457,7 @@
       </c>
       <c r="D440" t="inlineStr">
         <is>
-          <t>network,network property,cyber security,security protocol</t>
+          <t>network,network property,security,security protocol</t>
         </is>
       </c>
       <c r="E440" t="inlineStr">
@@ -19930,7 +19930,7 @@
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,51% attack,proof-of-work,proof-of-stake,dpos</t>
+          <t>blockchain,contract,51% attack,proof-of-work,proof-of-stake,dpos</t>
         </is>
       </c>
       <c r="E451" t="inlineStr">
@@ -20016,7 +20016,7 @@
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,peer-to-peer compute,fee,data model,reliability,ecosystem</t>
+          <t>blockchain,contract,peer-to-peer,fee,data model,reliability,ecosystem</t>
         </is>
       </c>
       <c r="E453" t="inlineStr">
@@ -20102,7 +20102,7 @@
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,supply chain,peer-to-peer compute,distribute ledger,systematics,bibliography</t>
+          <t>blockchain,contract,supply chain,peer-to-peer,distribute ledger,systematics,bibliography</t>
         </is>
       </c>
       <c r="E455" t="inlineStr">
@@ -20145,7 +20145,7 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>blockchain,medical service,scalability,systematics,peer-to-peer compute,database,data mine</t>
+          <t>blockchain,medical service,scalability,systematics,peer-to-peer,database,data mine</t>
         </is>
       </c>
       <c r="E456" t="inlineStr">
@@ -20188,7 +20188,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>blockchain,smart phone,peer-to-peer compute,task analysis,security,performance evaluation</t>
+          <t>blockchain,smart phone,peer-to-peer,task analysis,security,performance evaluation</t>
         </is>
       </c>
       <c r="E457" t="inlineStr">
@@ -20317,7 +20317,7 @@
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>blockchain,cyber security,ddos,bitcoin</t>
+          <t>blockchain,security,ddos,bitcoin</t>
         </is>
       </c>
       <c r="E460" t="inlineStr">
@@ -20532,7 +20532,7 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,distribute database,web server,file system,b,width,rout</t>
+          <t>peer-to-peer,distribute database,web server,file system,b,width,rout</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
@@ -20575,7 +20575,7 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>blockchain,security,peer-to-peer compute,software define network,computer architecture,software,control system</t>
+          <t>blockchain,security,peer-to-peer,software define network,computer architecture,software,control system</t>
         </is>
       </c>
       <c r="E466" t="inlineStr">
@@ -20704,7 +20704,7 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,publish,bitcoin,protocol</t>
+          <t>peer-to-peer,publish,bitcoin,protocol</t>
         </is>
       </c>
       <c r="E469" t="inlineStr">
@@ -20876,7 +20876,7 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>blockchain,distributed ledger technology,performance model,performance evaluation,systematic survey</t>
+          <t>blockchain,distribute ledger,performance model,performance evaluation,systematic survey</t>
         </is>
       </c>
       <c r="E473" t="inlineStr">
@@ -20919,7 +20919,7 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>consensus,peer-to-peer compute,industry,cloud compute,blockchain,security,ecosystem</t>
+          <t>consensus,peer-to-peer,industry,cloud compute,blockchain,security,ecosystem</t>
         </is>
       </c>
       <c r="E474" t="inlineStr">
@@ -21048,7 +21048,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>peer-to-peer compute,physical layer,price,energy management,blockchain,energy resource,australia</t>
+          <t>peer-to-peer,physical layer,price,energy management,blockchain,energy resource,australia</t>
         </is>
       </c>
       <c r="E477" t="inlineStr">
@@ -21091,7 +21091,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>bitcoin,blockchain,smart contract,smart contract application,smart contract operation,recent advance in smart contract</t>
+          <t>bitcoin,blockchain,contract,smart contract application,smart contract operation,recent advance in smart contract</t>
         </is>
       </c>
       <c r="E478" t="inlineStr">
@@ -21134,7 +21134,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>education,library,biological system model,adaptation model,peer-to-peer compute</t>
+          <t>education,library,biological system model,adaptation model,peer-to-peer</t>
         </is>
       </c>
       <c r="E479" t="inlineStr">
@@ -21177,7 +21177,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>internet of thing ,security,blockchain,ddos,ethereum,smart contract</t>
+          <t>internet of thing ,security,blockchain,ddos,ethereum,contract</t>
         </is>
       </c>
       <c r="E480" t="inlineStr">
@@ -21521,7 +21521,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>smart city,blockchain,security,privacy,consensus,smart contract,smart community</t>
+          <t>smart city,blockchain,security,privacy,consensus,contract,smart community</t>
         </is>
       </c>
       <c r="E488" t="inlineStr">
@@ -21650,7 +21650,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>internet of things,security,machine learn,artificial intelligence,technology</t>
+          <t>internet of things,security,machine learning,artificial intelligence,technology</t>
         </is>
       </c>
       <c r="E491" t="inlineStr">
@@ -22643,7 +22643,7 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,cryptocurrency,share resource,internet 3.0</t>
+          <t>blockchain,contract,cryptocurrency,share resource,internet 3.0</t>
         </is>
       </c>
       <c r="E514" t="inlineStr">
@@ -23034,7 +23034,7 @@
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,distribute registry,public procurement,electronic registration,international trade deal,к10,k15,k41,o38,l88</t>
+          <t>contract,blockchain,distribute registry,public procurement,electronic registration,international trade deal,к10,k15,k41,o38,l88</t>
         </is>
       </c>
       <c r="E523" t="inlineStr">
@@ -23253,7 +23253,7 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>blockchain,ttp,cyberattacks,decentralise,distributed ledger technology,artificial intelligence,internet of things</t>
+          <t>blockchain,ttp,cyberattacks,decentralise,distribute ledger,artificial intelligence,internet of things</t>
         </is>
       </c>
       <c r="E528" t="inlineStr">
@@ -23557,7 +23557,7 @@
       </c>
       <c r="D535" t="inlineStr">
         <is>
-          <t>blockchain,distribute ledger,smart contract,disruptive technology</t>
+          <t>blockchain,distribute ledger,contract,disruptive technology</t>
         </is>
       </c>
       <c r="E535" t="inlineStr">
@@ -23647,7 +23647,7 @@
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>blockchain,decentralize network,merkle tree,consensus,smart contract,hyperledger</t>
+          <t>blockchain,decentralize network,merkle tree,consensus,contract,hyperledger</t>
         </is>
       </c>
       <c r="E537" t="inlineStr">
@@ -23693,7 +23693,7 @@
       </c>
       <c r="D538" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,decentralization,immutable,data privacy</t>
+          <t>blockchain,contract,decentralization,immutable,data privacy</t>
         </is>
       </c>
       <c r="E538" t="inlineStr">
@@ -23736,7 +23736,7 @@
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>blockchain,cyber security,privacy,trust,cryptocurrency,cyberspace,smart contract,decentralization,peer-to-peer network,cyber security,protocol,cryptography</t>
+          <t>blockchain,security,privacy,trust,cryptocurrency,cyberspace,contract,decentralization,peer-to-peer network,security,protocol,cryptography</t>
         </is>
       </c>
       <c r="E539" t="inlineStr">
@@ -23869,7 +23869,7 @@
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>blockchain,industry 4.0,another keyword</t>
+          <t>blockchain,industry,another keyword</t>
         </is>
       </c>
       <c r="E542" t="inlineStr">
@@ -24229,7 +24229,7 @@
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>taxonomy,construction supply chain,threat model analysis,security level analysis,cyber security,vulnerability,smart contract,cyber attack</t>
+          <t>taxonomy,construction supply chain,threat model analysis,security level analysis,security,vulnerability,contract,cyber attack</t>
         </is>
       </c>
       <c r="E550" t="inlineStr">
@@ -24275,7 +24275,7 @@
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>smart contract,ethereum,blockchain</t>
+          <t>contract,ethereum,blockchain</t>
         </is>
       </c>
       <c r="E551" t="inlineStr">
@@ -24767,7 +24767,7 @@
       </c>
       <c r="D562" t="inlineStr">
         <is>
-          <t>blockchain,artificial intelligence,distribute ledger,machine learn,smart contract</t>
+          <t>blockchain,artificial intelligence,distribute ledger,machine learning,contract</t>
         </is>
       </c>
       <c r="E562" t="inlineStr">
@@ -24901,7 +24901,7 @@
       </c>
       <c r="D565" t="inlineStr">
         <is>
-          <t>reputation system,blockchain,smart contract,e-commerce,hyperledger</t>
+          <t>reputation system,blockchain,contract,e-commerce,hyperledger</t>
         </is>
       </c>
       <c r="E565" t="inlineStr">
@@ -25118,7 +25118,7 @@
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,evaluation framework,empirical evaluation</t>
+          <t>blockchain,contract,evaluation framework,empirical evaluation</t>
         </is>
       </c>
       <c r="E570" t="inlineStr">
@@ -25161,7 +25161,7 @@
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>tor,blockchain,cyber security,anonymity,privacy,cyber attack,onion service,pii,encryption,security</t>
+          <t>tor,blockchain,security,anonymity,privacy,cyber attack,onion service,pii,encryption,security</t>
         </is>
       </c>
       <c r="E571" t="inlineStr">
@@ -25594,7 +25594,7 @@
       </c>
       <c r="D581" t="inlineStr">
         <is>
-          <t>account,technology,bitcoin,cryptocurrency,cyber security,fraud,transparency</t>
+          <t>account,technology,bitcoin,cryptocurrency,security,fraud,transparency</t>
         </is>
       </c>
       <c r="E581" t="inlineStr">
@@ -25813,7 +25813,7 @@
       </c>
       <c r="D586" t="inlineStr">
         <is>
-          <t>blockchain,smart contract,supply chain,project management,construction</t>
+          <t>blockchain,contract,supply chain,project management,construction</t>
         </is>
       </c>
       <c r="E586" t="inlineStr">
@@ -25945,7 +25945,7 @@
       </c>
       <c r="D589" t="inlineStr">
         <is>
-          <t>blockchain,health 4.0,industry 4.0,decentralization,data management,trust,traceability,supply chain</t>
+          <t>blockchain,health 4.0,industry,decentralization,data management,trust,traceability,supply chain</t>
         </is>
       </c>
       <c r="E589" t="inlineStr">
@@ -26118,7 +26118,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>blockchain,certificate authority,cloud compute,public key infrastructure,smart contract,byzantine fault tolerance,state machine replication,partition,sharding</t>
+          <t>blockchain,certificate authority,cloud compute,public key infrastructure,contract,byzantine fault tolerance,state machine replication,partition,sharding</t>
         </is>
       </c>
       <c r="E593" t="inlineStr">
@@ -26297,7 +26297,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>blockchain,distribute ledger,bank industry,smart contract</t>
+          <t>blockchain,distribute ledger,bank industry,contract</t>
         </is>
       </c>
       <c r="E597" t="inlineStr">
@@ -26647,7 +26647,7 @@
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>blockchain,bpmn,business process,smart contract,temporal constraint,trust</t>
+          <t>blockchain,bpmn,business process,contract,temporal constraint,trust</t>
         </is>
       </c>
       <c r="E605" t="inlineStr">
@@ -26948,7 +26948,7 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>blockchain,cryptocurrency,energy consumption,distributed ledger technology,sustainability</t>
+          <t>blockchain,cryptocurrency,energy consumption,distribute ledger,sustainability</t>
         </is>
       </c>
       <c r="E612" t="inlineStr">
@@ -27256,7 +27256,7 @@
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>blockchain,security,cryptocurrency,smart contract</t>
+          <t>blockchain,security,cryptocurrency,contract</t>
         </is>
       </c>
       <c r="E619" t="inlineStr">
@@ -27299,7 +27299,7 @@
       </c>
       <c r="D620" t="inlineStr">
         <is>
-          <t>smart contract,blockchain,cryptocurrency,decentralization</t>
+          <t>contract,blockchain,cryptocurrency,decentralization</t>
         </is>
       </c>
       <c r="E620" t="inlineStr">
@@ -27342,7 +27342,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>5g network,blockchain,5g internet of thing,5g service,machine learn,security,privacy</t>
+          <t>5g network,blockchain,5g internet of thing,5g service,machine learning,security,privacy</t>
         </is>
       </c>
       <c r="E621" t="inlineStr">

</xml_diff>

<commit_message>
fix coincide bug and use // replace the #
</commit_message>
<xml_diff>
--- a/src/out/all-preprocessed.xlsx
+++ b/src/out/all-preprocessed.xlsx
@@ -8859,7 +8859,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>security,privacy,human and societal aspect of security and privacy,privacy protection,security service,system security,distribute system security</t>
+          <t>security,privacy,human and societal aspect of security and privacy,privacy protection,security service,system security,system security</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -19586,7 +19586,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>security,privacy,system security,distribute system security</t>
+          <t>security,privacy,system security,system security</t>
         </is>
       </c>
       <c r="E443" t="inlineStr">

</xml_diff>